<commit_message>
Finished Report, Cleaned up code, Fixed data
</commit_message>
<xml_diff>
--- a/Lab3/src/Data/TimingData.xlsx
+++ b/Lab3/src/Data/TimingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayso\Documents\College\CS_3353\Program3.0\Program3.0\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CA7288-44D7-4714-BF0F-D4D34658FBD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B31384-14A5-4C77-98D4-4B71D8EB15BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A732A4A-09F0-4824-967A-6CA6709296F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5A732A4A-09F0-4824-967A-6CA6709296F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -285,7 +285,100 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="36">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -5040,7 +5133,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50ED069D-38FD-4C34-AB9D-0A0EE2BA2135}" name="Table1" displayName="Table1" ref="B2:G12" headerRowDxfId="15" dataDxfId="27" totalsRowDxfId="14" headerRowBorderDxfId="19" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1CA167EF-D0B0-412B-9676-5304A24C5850}" name="Table3" displayName="Table3" ref="B1:D23" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="B1:D23" xr:uid="{8886D4AA-D507-401F-9F77-2A197F373981}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B6C6179B-FB72-4F29-A03B-DC61217FBE7C}" name="nodes" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DEDE1A01-12E0-4ED2-ACD9-96AF5C651C9A}" name="brute (sec)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{CF89B731-6558-48B5-B78E-7F64E5D8C7F3}" name="dynamic (sec)" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50ED069D-38FD-4C34-AB9D-0A0EE2BA2135}" name="Table1" displayName="Table1" ref="B2:G12" headerRowDxfId="23" dataDxfId="35" totalsRowDxfId="22" headerRowBorderDxfId="27" tableBorderDxfId="28">
   <autoFilter ref="B2:G12" xr:uid="{43D9832C-470B-435F-BAEF-C1A9C9F576E4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5050,16 +5159,16 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D566FB98-39DA-4A3F-9DD9-99E3200E0507}" name="nodes" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{384AA514-8AD8-4C1D-972F-F8564B4A9C04}" name="brute timing (sec)" dataDxfId="3" totalsRowDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{E22D48BD-CDCB-4C69-ABFB-15604A6323B3}" name="n! operations" dataDxfId="4" totalsRowDxfId="23">
+    <tableColumn id="1" xr3:uid="{D566FB98-39DA-4A3F-9DD9-99E3200E0507}" name="nodes" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{384AA514-8AD8-4C1D-972F-F8564B4A9C04}" name="brute timing (sec)" dataDxfId="11" totalsRowDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{E22D48BD-CDCB-4C69-ABFB-15604A6323B3}" name="n! operations" dataDxfId="12" totalsRowDxfId="31">
       <calculatedColumnFormula>FACT(B3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9714F496-047A-4D1B-BE80-DB5B0263F6F6}" name="n! avg" dataDxfId="18" totalsRowDxfId="24">
+    <tableColumn id="4" xr3:uid="{9714F496-047A-4D1B-BE80-DB5B0263F6F6}" name="n! avg" dataDxfId="26" totalsRowDxfId="32">
       <calculatedColumnFormula>C3/D3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3807D33E-E879-4D28-A375-AC49A4D647C8}" name="n! avg avg" dataDxfId="17" totalsRowDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{1076F956-3D92-4C01-9279-9F28B789BD80}" name="n! normailized" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="26">
+    <tableColumn id="5" xr3:uid="{3807D33E-E879-4D28-A375-AC49A4D647C8}" name="n! avg avg" dataDxfId="25" totalsRowDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{1076F956-3D92-4C01-9279-9F28B789BD80}" name="n! normailized" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="34">
       <calculatedColumnFormula>D3*F3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5067,8 +5176,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{944B448B-E284-44A5-A1F3-B1B177E5B84B}" name="Table2" displayName="Table2" ref="B2:G24" totalsRowShown="0" headerRowDxfId="6" dataDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{944B448B-E284-44A5-A1F3-B1B177E5B84B}" name="Table2" displayName="Table2" ref="B2:G24" totalsRowShown="0" headerRowDxfId="14" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20" totalsRowBorderDxfId="18">
   <autoFilter ref="B2:G24" xr:uid="{6E54B9AA-F5DC-4264-976F-4B9A3C83F429}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5078,16 +5187,16 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{974B226B-FB3D-4A20-94D9-B22683AC47BD}" name="nodes" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{571FB629-8889-4388-ACF3-EF0685CE75A0}" name="dynamic timing (sec)" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{9C92F401-E09D-4C6E-9ACF-CFEBC4AE820E}" name="2^n*n^2 operations" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{974B226B-FB3D-4A20-94D9-B22683AC47BD}" name="nodes" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{571FB629-8889-4388-ACF3-EF0685CE75A0}" name="dynamic timing (sec)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{9C92F401-E09D-4C6E-9ACF-CFEBC4AE820E}" name="2^n*n^2 operations" dataDxfId="9">
       <calculatedColumnFormula>POWER(B3,2) * POWER(2,B3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{491F6726-77BA-4C72-A8FB-25BDB353A1AA}" name="2^n*n^2 avg" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{491F6726-77BA-4C72-A8FB-25BDB353A1AA}" name="2^n*n^2 avg" dataDxfId="17">
       <calculatedColumnFormula>C3/D3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{81DB88CD-920B-4605-A019-37D213363F91}" name="2^n*n^2 avg avg" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{6FB90FC7-BBF0-4BDF-9E68-D28F5A1A3C9E}" name="2^n*n^2 normalized" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{81DB88CD-920B-4605-A019-37D213363F91}" name="2^n*n^2 avg avg" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{6FB90FC7-BBF0-4BDF-9E68-D28F5A1A3C9E}" name="2^n*n^2 normalized" dataDxfId="15">
       <calculatedColumnFormula>D3*F3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5394,15 +5503,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19BAA61-1940-4901-A6BE-45BED94490DE}">
   <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -5411,13 +5520,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
@@ -5434,13 +5543,13 @@
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2">
+      <c r="B2" s="5">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="6">
         <v>1.2619999999999999E-5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="8">
         <v>5.1579000000000002E-5</v>
       </c>
       <c r="F2">
@@ -5461,13 +5570,13 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="B3" s="5">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="7">
         <v>2.7160000000000001E-5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>9.4388000000000005E-5</v>
       </c>
       <c r="F3">
@@ -5488,13 +5597,13 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="B4" s="5">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>1.0665100000000001E-4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>1.77028E-4</v>
       </c>
       <c r="F4">
@@ -5515,13 +5624,13 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="5">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="7">
         <v>6.26018E-4</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>3.2695000000000001E-4</v>
       </c>
       <c r="F5">
@@ -5542,13 +5651,13 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="B6" s="5">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <v>4.7256199999999998E-3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <v>6.5628799999999999E-4</v>
       </c>
       <c r="F6">
@@ -5569,13 +5678,13 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="B7" s="5">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="7">
         <v>3.5930999999999998E-2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>1.22966E-3</v>
       </c>
       <c r="F7">
@@ -5596,13 +5705,13 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="B8" s="5">
         <v>10</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <v>0.211171</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>1.3134900000000001E-3</v>
       </c>
       <c r="F8">
@@ -5623,13 +5732,13 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="B9" s="5">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="7">
         <v>1.67526</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>2.9777200000000001E-3</v>
       </c>
       <c r="F9">
@@ -5650,13 +5759,13 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="B10" s="5">
         <v>12</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="7">
         <v>19.1431</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>6.7797100000000004E-3</v>
       </c>
       <c r="F10">
@@ -5677,13 +5786,13 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="B11" s="5">
         <v>13</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>242.07400000000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <v>1.5807399999999999E-2</v>
       </c>
       <c r="F11">
@@ -5704,10 +5813,11 @@
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="B12" s="5">
         <v>14</v>
       </c>
-      <c r="D12">
+      <c r="C12" s="7"/>
+      <c r="D12" s="8">
         <v>7.3806899999999995E-2</v>
       </c>
       <c r="G12">
@@ -5720,10 +5830,11 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="B13" s="5">
         <v>15</v>
       </c>
-      <c r="D13">
+      <c r="C13" s="7"/>
+      <c r="D13" s="8">
         <v>0.147539</v>
       </c>
       <c r="G13">
@@ -5736,10 +5847,11 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="B14" s="5">
         <v>16</v>
       </c>
-      <c r="D14">
+      <c r="C14" s="7"/>
+      <c r="D14" s="8">
         <v>0.302761</v>
       </c>
       <c r="G14">
@@ -5752,10 +5864,11 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="B15" s="5">
         <v>17</v>
       </c>
-      <c r="D15">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8">
         <v>0.63900500000000005</v>
       </c>
       <c r="G15">
@@ -5768,10 +5881,11 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="B16" s="5">
         <v>18</v>
       </c>
-      <c r="D16">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8">
         <v>1.5432399999999999</v>
       </c>
       <c r="G16">
@@ -5784,10 +5898,11 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="B17" s="5">
         <v>19</v>
       </c>
-      <c r="D17">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8">
         <v>3.0909399999999998</v>
       </c>
       <c r="G17">
@@ -5800,10 +5915,11 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="B18" s="5">
         <v>20</v>
       </c>
-      <c r="D18">
+      <c r="C18" s="7"/>
+      <c r="D18" s="8">
         <v>6.4703600000000003</v>
       </c>
       <c r="G18">
@@ -5816,10 +5932,11 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="B19" s="5">
         <v>21</v>
       </c>
-      <c r="D19">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8">
         <v>14.057499999999999</v>
       </c>
       <c r="G19">
@@ -5832,10 +5949,11 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="B20" s="5">
         <v>22</v>
       </c>
-      <c r="D20">
+      <c r="C20" s="7"/>
+      <c r="D20" s="8">
         <v>30.588999999999999</v>
       </c>
       <c r="G20">
@@ -5848,10 +5966,11 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21">
+      <c r="B21" s="5">
         <v>23</v>
       </c>
-      <c r="D21">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8">
         <v>66.254499999999993</v>
       </c>
       <c r="G21">
@@ -5864,10 +5983,11 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="B22" s="5">
         <v>24</v>
       </c>
-      <c r="D22">
+      <c r="C22" s="7"/>
+      <c r="D22" s="8">
         <v>144.99299999999999</v>
       </c>
       <c r="G22">
@@ -5880,10 +6000,11 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="B23" s="9">
         <v>25</v>
       </c>
-      <c r="D23">
+      <c r="C23" s="10"/>
+      <c r="D23" s="11">
         <v>315.95999999999998</v>
       </c>
       <c r="G23">
@@ -6101,6 +6222,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -6109,7 +6233,7 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6395,8 +6519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1CA1E0-591C-4195-8C1D-BEE81507D8DE}">
   <dimension ref="B2:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>